<commit_message>
small fix in test cases sheet
</commit_message>
<xml_diff>
--- a/Unit Tests/Mcal/Atmega32/UART/TestCases.xlsx
+++ b/Unit Tests/Mcal/Atmega32/UART/TestCases.xlsx
@@ -5,10 +5,10 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\Unit Tests\Mcal\Atmega32\UART\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\sprints-2021\Unit Tests\Mcal\Atmega32\UART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660FC1A9-84CA-4646-A793-9FA8039325A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52E5B956-8E46-411D-BB8F-CE8712651329}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56237F82-C67E-4D5F-9511-A6B1695E74E7}"/>
   </bookViews>
@@ -346,9 +346,7 @@
     <tableColumn id="2" xr3:uid="{20E110E4-5360-4262-BEC4-A07BEF421B26}" name="Test Summary"/>
     <tableColumn id="3" xr3:uid="{1E5A2B7F-0EE5-497D-B5A1-FD09AE1F0DDA}" name="Expected Result"/>
     <tableColumn id="4" xr3:uid="{5F7F029B-8ED5-4221-846F-88EEC85FF0D6}" name="PASSED/FAILED"/>
-    <tableColumn id="5" xr3:uid="{D2FEDBB2-0E1E-43ED-8BA8-7FBCF07B2E18}" name="Last Runtime" dataDxfId="0">
-      <calculatedColumnFormula>TODAY()</calculatedColumnFormula>
-    </tableColumn>
+    <tableColumn id="5" xr3:uid="{D2FEDBB2-0E1E-43ED-8BA8-7FBCF07B2E18}" name="Last Runtime" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="TableStyleMedium14" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -653,8 +651,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E4C935-3205-4223-8F2E-9D124BD53C3F}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="E2" sqref="E2:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -698,7 +696,6 @@
         <v>52</v>
       </c>
       <c r="E2" s="1">
-        <f ca="1">TODAY()</f>
         <v>44412</v>
       </c>
       <c r="F2" s="1"/>
@@ -717,7 +714,6 @@
         <v>52</v>
       </c>
       <c r="E3" s="1">
-        <f ca="1">TODAY()</f>
         <v>44412</v>
       </c>
       <c r="F3" s="1"/>
@@ -736,7 +732,6 @@
         <v>52</v>
       </c>
       <c r="E4" s="1">
-        <f ca="1">TODAY()</f>
         <v>44412</v>
       </c>
       <c r="F4" s="1"/>
@@ -755,7 +750,6 @@
         <v>52</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:F35" ca="1" si="0">TODAY()</f>
         <v>44412</v>
       </c>
       <c r="F5" s="1"/>
@@ -774,7 +768,6 @@
         <v>52</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F6" s="1"/>
@@ -793,7 +786,6 @@
         <v>52</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F7" s="1"/>
@@ -812,7 +804,6 @@
         <v>52</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F8" s="1"/>
@@ -831,7 +822,6 @@
         <v>52</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F9" s="1"/>
@@ -850,7 +840,6 @@
         <v>52</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F10" s="1"/>
@@ -869,7 +858,6 @@
         <v>52</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F11" s="1"/>
@@ -888,7 +876,6 @@
         <v>52</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F12" s="1"/>
@@ -907,7 +894,6 @@
         <v>52</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F13" s="1"/>
@@ -926,7 +912,6 @@
         <v>52</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F14" s="1"/>
@@ -945,7 +930,6 @@
         <v>52</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F15" s="1"/>
@@ -964,7 +948,6 @@
         <v>52</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F16" s="1"/>
@@ -983,7 +966,6 @@
         <v>52</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F17" s="1"/>
@@ -1002,7 +984,6 @@
         <v>52</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F18" s="1"/>
@@ -1021,7 +1002,6 @@
         <v>52</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F19" s="1"/>
@@ -1040,7 +1020,6 @@
         <v>52</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F20" s="1"/>
@@ -1059,7 +1038,6 @@
         <v>52</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F21" s="1"/>
@@ -1078,7 +1056,6 @@
         <v>52</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F22" s="1"/>
@@ -1097,7 +1074,6 @@
         <v>52</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F23" s="1"/>
@@ -1116,7 +1092,6 @@
         <v>52</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F24" s="1"/>
@@ -1135,7 +1110,6 @@
         <v>52</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F25" s="1"/>
@@ -1154,7 +1128,6 @@
         <v>52</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F26" s="1"/>
@@ -1173,7 +1146,6 @@
         <v>52</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F27" s="1"/>
@@ -1192,7 +1164,6 @@
         <v>52</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F28" s="1"/>
@@ -1211,7 +1182,6 @@
         <v>52</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F29" s="1"/>
@@ -1230,7 +1200,6 @@
         <v>52</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F30" s="1"/>
@@ -1249,7 +1218,6 @@
         <v>52</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F31" s="1"/>
@@ -1268,7 +1236,6 @@
         <v>52</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F32" s="1"/>
@@ -1287,7 +1254,6 @@
         <v>52</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F33" s="1"/>
@@ -1306,7 +1272,6 @@
         <v>52</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F34" s="1"/>
@@ -1325,7 +1290,6 @@
         <v>52</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" ca="1" si="0"/>
         <v>44412</v>
       </c>
       <c r="F35" s="1"/>

</xml_diff>

<commit_message>
Small Fixes after Merging Sprint 2 and Sprint 3
</commit_message>
<xml_diff>
--- a/Unit Tests/Mcal/Atmega32/UART/TestCases.xlsx
+++ b/Unit Tests/Mcal/Atmega32/UART/TestCases.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24228"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="24326"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\Unit Tests\Mcal\Atmega32\UART\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="H:\Mohamed Sprints\sprints-2021\Unit Tests\Mcal\Atmega32\UART\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{660FC1A9-84CA-4646-A793-9FA8039325A9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{9CE9564E-CAB9-4D32-BFB1-E764416BF09D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{56237F82-C67E-4D5F-9511-A6B1695E74E7}"/>
   </bookViews>
@@ -653,8 +653,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{10E4C935-3205-4223-8F2E-9D124BD53C3F}">
   <dimension ref="A1:F35"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="B41" sqref="B41"/>
+    <sheetView tabSelected="1" topLeftCell="A9" workbookViewId="0">
+      <selection activeCell="E4" sqref="E4:E35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8" x14ac:dyDescent="0.25"/>
@@ -699,7 +699,7 @@
       </c>
       <c r="E2" s="1">
         <f ca="1">TODAY()</f>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F2" s="1"/>
     </row>
@@ -718,7 +718,7 @@
       </c>
       <c r="E3" s="1">
         <f ca="1">TODAY()</f>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F3" s="1"/>
     </row>
@@ -736,8 +736,7 @@
         <v>52</v>
       </c>
       <c r="E4" s="1">
-        <f ca="1">TODAY()</f>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F4" s="1"/>
     </row>
@@ -755,8 +754,7 @@
         <v>52</v>
       </c>
       <c r="E5" s="1">
-        <f t="shared" ref="E5:F35" ca="1" si="0">TODAY()</f>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F5" s="1"/>
     </row>
@@ -774,8 +772,7 @@
         <v>52</v>
       </c>
       <c r="E6" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F6" s="1"/>
     </row>
@@ -793,8 +790,7 @@
         <v>52</v>
       </c>
       <c r="E7" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F7" s="1"/>
     </row>
@@ -812,8 +808,7 @@
         <v>52</v>
       </c>
       <c r="E8" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F8" s="1"/>
     </row>
@@ -831,8 +826,7 @@
         <v>52</v>
       </c>
       <c r="E9" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F9" s="1"/>
     </row>
@@ -850,8 +844,7 @@
         <v>52</v>
       </c>
       <c r="E10" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F10" s="1"/>
     </row>
@@ -869,8 +862,7 @@
         <v>52</v>
       </c>
       <c r="E11" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F11" s="1"/>
     </row>
@@ -888,8 +880,7 @@
         <v>52</v>
       </c>
       <c r="E12" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F12" s="1"/>
     </row>
@@ -907,8 +898,7 @@
         <v>52</v>
       </c>
       <c r="E13" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F13" s="1"/>
     </row>
@@ -926,8 +916,7 @@
         <v>52</v>
       </c>
       <c r="E14" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F14" s="1"/>
     </row>
@@ -945,8 +934,7 @@
         <v>52</v>
       </c>
       <c r="E15" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F15" s="1"/>
     </row>
@@ -964,8 +952,7 @@
         <v>52</v>
       </c>
       <c r="E16" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F16" s="1"/>
     </row>
@@ -983,8 +970,7 @@
         <v>52</v>
       </c>
       <c r="E17" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F17" s="1"/>
     </row>
@@ -1002,8 +988,7 @@
         <v>52</v>
       </c>
       <c r="E18" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F18" s="1"/>
     </row>
@@ -1021,8 +1006,7 @@
         <v>52</v>
       </c>
       <c r="E19" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F19" s="1"/>
     </row>
@@ -1040,8 +1024,7 @@
         <v>52</v>
       </c>
       <c r="E20" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F20" s="1"/>
     </row>
@@ -1059,8 +1042,7 @@
         <v>52</v>
       </c>
       <c r="E21" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F21" s="1"/>
     </row>
@@ -1078,8 +1060,7 @@
         <v>52</v>
       </c>
       <c r="E22" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F22" s="1"/>
     </row>
@@ -1097,8 +1078,7 @@
         <v>52</v>
       </c>
       <c r="E23" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F23" s="1"/>
     </row>
@@ -1116,8 +1096,7 @@
         <v>52</v>
       </c>
       <c r="E24" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F24" s="1"/>
     </row>
@@ -1135,8 +1114,7 @@
         <v>52</v>
       </c>
       <c r="E25" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F25" s="1"/>
     </row>
@@ -1154,8 +1132,7 @@
         <v>52</v>
       </c>
       <c r="E26" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F26" s="1"/>
     </row>
@@ -1173,8 +1150,7 @@
         <v>52</v>
       </c>
       <c r="E27" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F27" s="1"/>
     </row>
@@ -1192,8 +1168,7 @@
         <v>52</v>
       </c>
       <c r="E28" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F28" s="1"/>
     </row>
@@ -1211,8 +1186,7 @@
         <v>52</v>
       </c>
       <c r="E29" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F29" s="1"/>
     </row>
@@ -1230,8 +1204,7 @@
         <v>52</v>
       </c>
       <c r="E30" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F30" s="1"/>
     </row>
@@ -1249,8 +1222,7 @@
         <v>52</v>
       </c>
       <c r="E31" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F31" s="1"/>
     </row>
@@ -1268,8 +1240,7 @@
         <v>52</v>
       </c>
       <c r="E32" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F32" s="1"/>
     </row>
@@ -1287,8 +1258,7 @@
         <v>52</v>
       </c>
       <c r="E33" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F33" s="1"/>
     </row>
@@ -1306,8 +1276,7 @@
         <v>52</v>
       </c>
       <c r="E34" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F34" s="1"/>
     </row>
@@ -1325,8 +1294,7 @@
         <v>52</v>
       </c>
       <c r="E35" s="1">
-        <f t="shared" ca="1" si="0"/>
-        <v>44412</v>
+        <v>44422</v>
       </c>
       <c r="F35" s="1"/>
     </row>

</xml_diff>